<commit_message>
updates about CSI493 test bug of scoring
</commit_message>
<xml_diff>
--- a/scoring/tests/CSI4/CSI493_test_1.xlsx
+++ b/scoring/tests/CSI4/CSI493_test_1.xlsx
@@ -440,7 +440,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -450,7 +450,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -460,7 +460,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -490,7 +490,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -520,7 +520,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -530,7 +530,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -540,7 +540,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -560,7 +560,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -580,7 +580,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -610,7 +610,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -620,7 +620,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -630,7 +630,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -640,7 +640,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -660,7 +660,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -670,7 +670,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -680,7 +680,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -720,7 +720,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -740,7 +740,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -760,7 +760,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -830,7 +830,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -840,7 +840,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -850,7 +850,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -860,7 +860,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -870,7 +870,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -890,7 +890,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -900,7 +900,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -930,7 +930,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -950,7 +950,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -960,7 +960,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -970,7 +970,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -980,7 +980,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1050,7 +1050,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1170,7 +1170,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1250,7 +1250,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1260,7 +1260,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1290,7 +1290,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1310,7 +1310,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1370,7 +1370,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1470,7 +1470,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -1758,27 +1758,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>dysthymia_total</t>
+          <t>dysthymia_type_a</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>autistic_disorder_type_a</t>
+          <t>dysthymia_type_b</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>autistic_disorder_type_b</t>
+          <t>dysthymia_total</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1788,7 +1788,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>autistic_disorder_type_c</t>
+          <t>autistic_disorder_type_a</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1798,17 +1798,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>autistic_disorder_total</t>
+          <t>autistic_disorder_type_b</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>asperger_disorder_type_a</t>
+          <t>autistic_disorder_type_c</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1818,71 +1818,71 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>asperger_disorder_type_b</t>
+          <t>autistic_disorder_total</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>asperger_disorder_total</t>
+          <t>asperger_disorder_type_a</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>social_phobia</t>
+          <t>asperger_disorder_type_b</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>seperation_anxiety_disorder</t>
+          <t>asperger_disorder_total</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>enuresis</t>
+          <t>social_phobia</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>dysthymia_type_a</t>
+          <t>seperation_anxiety_disorder</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>dysthymia_type_b</t>
+          <t>enuresis</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1922,7 +1922,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1982,7 +1982,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -2032,7 +2032,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -2042,7 +2042,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>